<commit_message>
interactive graph: year and woc
</commit_message>
<xml_diff>
--- a/data_output/data_overlap.xlsx
+++ b/data_output/data_overlap.xlsx
@@ -1219,7 +1219,7 @@
     </row>
     <row r="12">
       <c r="A12" s="1" t="n">
-        <v>1390</v>
+        <v>1394</v>
       </c>
       <c r="B12" t="inlineStr">
         <is>
@@ -1295,7 +1295,7 @@
     </row>
     <row r="13">
       <c r="A13" s="1" t="n">
-        <v>1391</v>
+        <v>1395</v>
       </c>
       <c r="B13" t="inlineStr">
         <is>
@@ -1371,7 +1371,7 @@
     </row>
     <row r="14">
       <c r="A14" s="1" t="n">
-        <v>1392</v>
+        <v>1396</v>
       </c>
       <c r="B14" t="inlineStr">
         <is>
@@ -1447,7 +1447,7 @@
     </row>
     <row r="15">
       <c r="A15" s="1" t="n">
-        <v>1595</v>
+        <v>1599</v>
       </c>
       <c r="B15" t="inlineStr">
         <is>
@@ -1523,7 +1523,7 @@
     </row>
     <row r="16">
       <c r="A16" s="1" t="n">
-        <v>1596</v>
+        <v>1600</v>
       </c>
       <c r="B16" t="inlineStr">
         <is>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="17">
       <c r="A17" s="1" t="n">
-        <v>1601</v>
+        <v>1605</v>
       </c>
       <c r="B17" t="inlineStr">
         <is>
@@ -1675,7 +1675,7 @@
     </row>
     <row r="18">
       <c r="A18" s="1" t="n">
-        <v>1602</v>
+        <v>1606</v>
       </c>
       <c r="B18" t="inlineStr">
         <is>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="19">
       <c r="A19" s="1" t="n">
-        <v>1903</v>
+        <v>1909</v>
       </c>
       <c r="B19" t="inlineStr">
         <is>
@@ -1827,7 +1827,7 @@
     </row>
     <row r="20">
       <c r="A20" s="1" t="n">
-        <v>1904</v>
+        <v>1910</v>
       </c>
       <c r="B20" t="inlineStr">
         <is>
@@ -1903,7 +1903,7 @@
     </row>
     <row r="21">
       <c r="A21" s="1" t="n">
-        <v>1905</v>
+        <v>1911</v>
       </c>
       <c r="B21" t="inlineStr">
         <is>
@@ -1979,7 +1979,7 @@
     </row>
     <row r="22">
       <c r="A22" s="1" t="n">
-        <v>2520</v>
+        <v>2526</v>
       </c>
       <c r="B22" t="inlineStr">
         <is>
@@ -2055,7 +2055,7 @@
     </row>
     <row r="23">
       <c r="A23" s="1" t="n">
-        <v>2521</v>
+        <v>2527</v>
       </c>
       <c r="B23" t="inlineStr">
         <is>
@@ -2131,7 +2131,7 @@
     </row>
     <row r="24">
       <c r="A24" s="1" t="n">
-        <v>2855</v>
+        <v>2863</v>
       </c>
       <c r="B24" t="inlineStr">
         <is>
@@ -2207,7 +2207,7 @@
     </row>
     <row r="25">
       <c r="A25" s="1" t="n">
-        <v>2856</v>
+        <v>2864</v>
       </c>
       <c r="B25" t="inlineStr">
         <is>
@@ -2283,7 +2283,7 @@
     </row>
     <row r="26">
       <c r="A26" s="1" t="n">
-        <v>2857</v>
+        <v>2865</v>
       </c>
       <c r="B26" t="inlineStr">
         <is>
@@ -2359,7 +2359,7 @@
     </row>
     <row r="27">
       <c r="A27" s="1" t="n">
-        <v>4085</v>
+        <v>4093</v>
       </c>
       <c r="B27" t="inlineStr">
         <is>
@@ -2435,7 +2435,7 @@
     </row>
     <row r="28">
       <c r="A28" s="1" t="n">
-        <v>4086</v>
+        <v>4094</v>
       </c>
       <c r="B28" t="inlineStr">
         <is>
@@ -2511,7 +2511,7 @@
     </row>
     <row r="29">
       <c r="A29" s="1" t="n">
-        <v>4087</v>
+        <v>4095</v>
       </c>
       <c r="B29" t="inlineStr">
         <is>
@@ -2587,7 +2587,7 @@
     </row>
     <row r="30">
       <c r="A30" s="1" t="n">
-        <v>4181</v>
+        <v>4189</v>
       </c>
       <c r="B30" t="inlineStr">
         <is>
@@ -2663,7 +2663,7 @@
     </row>
     <row r="31">
       <c r="A31" s="1" t="n">
-        <v>4182</v>
+        <v>4190</v>
       </c>
       <c r="B31" t="inlineStr">
         <is>
@@ -2739,7 +2739,7 @@
     </row>
     <row r="32">
       <c r="A32" s="1" t="n">
-        <v>4664</v>
+        <v>4675</v>
       </c>
       <c r="B32" t="inlineStr">
         <is>
@@ -2815,7 +2815,7 @@
     </row>
     <row r="33">
       <c r="A33" s="1" t="n">
-        <v>4665</v>
+        <v>4676</v>
       </c>
       <c r="B33" t="inlineStr">
         <is>
@@ -2891,7 +2891,7 @@
     </row>
     <row r="34">
       <c r="A34" s="1" t="n">
-        <v>4666</v>
+        <v>4677</v>
       </c>
       <c r="B34" t="inlineStr">
         <is>
@@ -2967,7 +2967,7 @@
     </row>
     <row r="35">
       <c r="A35" s="1" t="n">
-        <v>4762</v>
+        <v>4773</v>
       </c>
       <c r="B35" t="inlineStr">
         <is>
@@ -3043,7 +3043,7 @@
     </row>
     <row r="36">
       <c r="A36" s="1" t="n">
-        <v>4763</v>
+        <v>4774</v>
       </c>
       <c r="B36" t="inlineStr">
         <is>
@@ -3119,7 +3119,7 @@
     </row>
     <row r="37">
       <c r="A37" s="1" t="n">
-        <v>5220</v>
+        <v>5231</v>
       </c>
       <c r="B37" t="inlineStr">
         <is>
@@ -3195,7 +3195,7 @@
     </row>
     <row r="38">
       <c r="A38" s="1" t="n">
-        <v>5221</v>
+        <v>5232</v>
       </c>
       <c r="B38" t="inlineStr">
         <is>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="39">
       <c r="A39" s="1" t="n">
-        <v>5404</v>
+        <v>5415</v>
       </c>
       <c r="B39" t="inlineStr">
         <is>
@@ -3347,7 +3347,7 @@
     </row>
     <row r="40">
       <c r="A40" s="1" t="n">
-        <v>5405</v>
+        <v>5416</v>
       </c>
       <c r="B40" t="inlineStr">
         <is>
@@ -3423,7 +3423,7 @@
     </row>
     <row r="41">
       <c r="A41" s="1" t="n">
-        <v>5469</v>
+        <v>5480</v>
       </c>
       <c r="B41" t="inlineStr">
         <is>
@@ -3499,7 +3499,7 @@
     </row>
     <row r="42">
       <c r="A42" s="1" t="n">
-        <v>5470</v>
+        <v>5481</v>
       </c>
       <c r="B42" t="inlineStr">
         <is>
@@ -3575,7 +3575,7 @@
     </row>
     <row r="43">
       <c r="A43" s="1" t="n">
-        <v>5660</v>
+        <v>5671</v>
       </c>
       <c r="B43" t="inlineStr">
         <is>
@@ -3651,7 +3651,7 @@
     </row>
     <row r="44">
       <c r="A44" s="1" t="n">
-        <v>5661</v>
+        <v>5672</v>
       </c>
       <c r="B44" t="inlineStr">
         <is>
@@ -3727,7 +3727,7 @@
     </row>
     <row r="45">
       <c r="A45" s="1" t="n">
-        <v>5853</v>
+        <v>5864</v>
       </c>
       <c r="B45" t="inlineStr">
         <is>
@@ -3803,7 +3803,7 @@
     </row>
     <row r="46">
       <c r="A46" s="1" t="n">
-        <v>5854</v>
+        <v>5865</v>
       </c>
       <c r="B46" t="inlineStr">
         <is>
@@ -3879,7 +3879,7 @@
     </row>
     <row r="47">
       <c r="A47" s="1" t="n">
-        <v>5983</v>
+        <v>5996</v>
       </c>
       <c r="B47" t="inlineStr">
         <is>
@@ -3955,7 +3955,7 @@
     </row>
     <row r="48">
       <c r="A48" s="1" t="n">
-        <v>5984</v>
+        <v>5997</v>
       </c>
       <c r="B48" t="inlineStr">
         <is>
@@ -4031,7 +4031,7 @@
     </row>
     <row r="49">
       <c r="A49" s="1" t="n">
-        <v>6020</v>
+        <v>6033</v>
       </c>
       <c r="B49" t="inlineStr">
         <is>
@@ -4107,7 +4107,7 @@
     </row>
     <row r="50">
       <c r="A50" s="1" t="n">
-        <v>6021</v>
+        <v>6034</v>
       </c>
       <c r="B50" t="inlineStr">
         <is>
@@ -4183,7 +4183,7 @@
     </row>
     <row r="51">
       <c r="A51" s="1" t="n">
-        <v>6022</v>
+        <v>6035</v>
       </c>
       <c r="B51" t="inlineStr">
         <is>
@@ -4259,7 +4259,7 @@
     </row>
     <row r="52">
       <c r="A52" s="1" t="n">
-        <v>6223</v>
+        <v>6236</v>
       </c>
       <c r="B52" t="inlineStr">
         <is>
@@ -4335,7 +4335,7 @@
     </row>
     <row r="53">
       <c r="A53" s="1" t="n">
-        <v>6224</v>
+        <v>6237</v>
       </c>
       <c r="B53" t="inlineStr">
         <is>
@@ -4411,7 +4411,7 @@
     </row>
     <row r="54">
       <c r="A54" s="1" t="n">
-        <v>6493</v>
+        <v>6508</v>
       </c>
       <c r="B54" t="inlineStr">
         <is>
@@ -4487,7 +4487,7 @@
     </row>
     <row r="55">
       <c r="A55" s="1" t="n">
-        <v>6494</v>
+        <v>6509</v>
       </c>
       <c r="B55" t="inlineStr">
         <is>
@@ -4563,7 +4563,7 @@
     </row>
     <row r="56">
       <c r="A56" s="1" t="n">
-        <v>6591</v>
+        <v>6606</v>
       </c>
       <c r="B56" t="inlineStr">
         <is>
@@ -4639,7 +4639,7 @@
     </row>
     <row r="57">
       <c r="A57" s="1" t="n">
-        <v>6592</v>
+        <v>6607</v>
       </c>
       <c r="B57" t="inlineStr">
         <is>
@@ -4715,7 +4715,7 @@
     </row>
     <row r="58">
       <c r="A58" s="1" t="n">
-        <v>7313</v>
+        <v>7328</v>
       </c>
       <c r="B58" t="inlineStr">
         <is>
@@ -4791,7 +4791,7 @@
     </row>
     <row r="59">
       <c r="A59" s="1" t="n">
-        <v>7314</v>
+        <v>7329</v>
       </c>
       <c r="B59" t="inlineStr">
         <is>
@@ -4867,7 +4867,7 @@
     </row>
     <row r="60">
       <c r="A60" s="1" t="n">
-        <v>7803</v>
+        <v>7820</v>
       </c>
       <c r="B60" t="inlineStr">
         <is>
@@ -4943,7 +4943,7 @@
     </row>
     <row r="61">
       <c r="A61" s="1" t="n">
-        <v>7804</v>
+        <v>7821</v>
       </c>
       <c r="B61" t="inlineStr">
         <is>

</xml_diff>